<commit_message>
VIEW: shoot, projection -> kinesis
</commit_message>
<xml_diff>
--- a/src/main/others/FairyList.xlsx
+++ b/src/main/others/FairyList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CDC489-9724-475C-A0C1-657B0F3D5951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B11068-02C8-4A04-B3BB-33FDC28F98D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7395" yWindow="1290" windowWidth="20325" windowHeight="14115" xr2:uid="{50F21D03-37BB-40FB-A570-1AD8030E22E9}"/>
   </bookViews>
@@ -2607,12 +2607,6 @@
     <t>空間</t>
   </si>
   <si>
-    <t>縮地</t>
-  </si>
-  <si>
-    <t>射出</t>
-  </si>
-  <si>
     <t>破壊</t>
   </si>
   <si>
@@ -4569,6 +4563,17 @@
   </si>
   <si>
     <t>flower_picking_bell</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>縮地</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>運動</t>
+    <rPh sb="0" eb="2">
+      <t>ウンドウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5335,7 +5340,7 @@
     <tableColumn id="25" xr3:uid="{3CFDC570-BDAB-4914-ABC3-2C36BC441EFF}" name="音波" dataDxfId="25"/>
     <tableColumn id="27" xr3:uid="{57B5D258-645E-405C-8646-A5BA9977E94A}" name="空間" dataDxfId="24"/>
     <tableColumn id="28" xr3:uid="{FC7CB677-4A50-4B6E-A9B9-30E79C62F98D}" name="縮地" dataDxfId="23"/>
-    <tableColumn id="29" xr3:uid="{0A208B09-58DF-41DC-8C05-5263F315034B}" name="射出" dataDxfId="22"/>
+    <tableColumn id="29" xr3:uid="{0A208B09-58DF-41DC-8C05-5263F315034B}" name="運動" dataDxfId="22"/>
     <tableColumn id="31" xr3:uid="{B7C69519-DEF6-4AE2-A3F5-853F5A3D600F}" name="破壊" dataDxfId="21"/>
     <tableColumn id="32" xr3:uid="{EF23F12F-E8B4-4880-9CA7-0217FC0413E6}" name="化学" dataDxfId="20"/>
     <tableColumn id="33" xr3:uid="{D40F96E4-B2C9-4D5D-AB4C-D11CBE93B14C}" name="切断" dataDxfId="19"/>
@@ -5631,10 +5636,10 @@
   <dimension ref="A1:BC214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="Y86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H168" sqref="H168"/>
+      <selection pane="bottomRight" activeCell="AM94" sqref="AM94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5681,7 +5686,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>160</v>
@@ -5717,7 +5722,7 @@
         <v>22</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="V1" s="14" t="s">
         <v>30</v>
@@ -5762,64 +5767,64 @@
         <v>592</v>
       </c>
       <c r="AJ1" s="14" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="AK1" s="14" t="s">
         <v>593</v>
       </c>
       <c r="AL1" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>984</v>
+      </c>
+      <c r="AN1" s="14" t="s">
         <v>594</v>
       </c>
-      <c r="AM1" s="14" t="s">
+      <c r="AO1" s="14" t="s">
         <v>595</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AP1" s="14" t="s">
         <v>596</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AQ1" s="14" t="s">
+        <v>692</v>
+      </c>
+      <c r="AR1" s="14" t="s">
         <v>597</v>
       </c>
-      <c r="AP1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>598</v>
       </c>
-      <c r="AQ1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="AU1" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="AW1" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="AY1" s="14" t="s">
         <v>694</v>
-      </c>
-      <c r="AR1" s="14" t="s">
-        <v>599</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>600</v>
-      </c>
-      <c r="AT1" s="14" t="s">
-        <v>601</v>
-      </c>
-      <c r="AU1" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="AV1" s="14" t="s">
-        <v>603</v>
-      </c>
-      <c r="AW1" s="14" t="s">
-        <v>604</v>
-      </c>
-      <c r="AX1" s="14" t="s">
-        <v>695</v>
-      </c>
-      <c r="AY1" s="14" t="s">
-        <v>696</v>
       </c>
       <c r="AZ1" s="14" t="s">
         <v>426</v>
       </c>
       <c r="BA1" s="2" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.15">
@@ -5848,10 +5853,10 @@
         <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="K2" s="3">
         <v>1</v>
@@ -5990,7 +5995,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>125</v>
@@ -6138,7 +6143,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>127</v>
@@ -6440,7 +6445,7 @@
         <v>97</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>177</v>
@@ -6580,7 +6585,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>126</v>
@@ -6718,7 +6723,7 @@
         <v>91</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>172</v>
@@ -6866,10 +6871,10 @@
         <v>93</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="K9" s="3">
         <v>4</v>
@@ -7018,7 +7023,7 @@
         <v>96</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>163</v>
@@ -7170,7 +7175,7 @@
         <v>122</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>180</v>
@@ -7484,7 +7489,7 @@
         <v>98</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J13" s="10" t="s">
         <v>168</v>
@@ -7624,7 +7629,7 @@
         <v>92</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>572</v>
@@ -7774,10 +7779,10 @@
         <v>105</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="K15" s="3">
         <v>2</v>
@@ -7911,7 +7916,7 @@
         <v>229</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>44</v>
@@ -7926,7 +7931,7 @@
         <v>104</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>167</v>
@@ -8071,7 +8076,7 @@
         <v>229</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>42</v>
@@ -8086,10 +8091,10 @@
         <v>102</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="K17" s="3">
         <v>1</v>
@@ -8229,7 +8234,7 @@
         <v>229</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>43</v>
@@ -8244,7 +8249,7 @@
         <v>103</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>175</v>
@@ -8400,7 +8405,7 @@
         <v>106</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>179</v>
@@ -8538,7 +8543,7 @@
         <v>101</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>174</v>
@@ -8680,7 +8685,7 @@
         <v>108</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>254</v>
@@ -8828,13 +8833,13 @@
         <v>309</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>166</v>
@@ -8982,7 +8987,7 @@
         <v>114</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>161</v>
@@ -9122,13 +9127,13 @@
         <v>311</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>99</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>252</v>
@@ -9268,7 +9273,7 @@
         <v>94</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>251</v>
@@ -9414,7 +9419,7 @@
         <v>95</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>171</v>
@@ -9542,7 +9547,7 @@
         <v>242</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>406</v>
@@ -9551,10 +9556,10 @@
         <v>123</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>181</v>
@@ -9695,19 +9700,19 @@
         <v>229</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>314</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>44</v>
@@ -9853,7 +9858,7 @@
         <v>229</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>60</v>
@@ -9868,7 +9873,7 @@
         <v>121</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>178</v>
@@ -10030,7 +10035,7 @@
         <v>115</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J30" s="10" t="s">
         <v>169</v>
@@ -10188,7 +10193,7 @@
         <v>249</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J31" s="10" t="s">
         <v>250</v>
@@ -10338,7 +10343,7 @@
         <v>109</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J32" s="10" t="s">
         <v>256</v>
@@ -10476,7 +10481,7 @@
         <v>245</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>401</v>
@@ -10485,10 +10490,10 @@
         <v>547</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>255</v>
@@ -10620,7 +10625,7 @@
         <v>107</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>570</v>
@@ -11178,7 +11183,7 @@
         <v>117</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J38" s="10" t="s">
         <v>183</v>
@@ -11320,7 +11325,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J39" s="10" t="s">
         <v>170</v>
@@ -11453,7 +11458,7 @@
         <v>232</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>49</v>
@@ -11468,7 +11473,7 @@
         <v>110</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>173</v>
@@ -11593,7 +11598,7 @@
         <v>232</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>50</v>
@@ -11608,7 +11613,7 @@
         <v>111</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J41" s="10" t="s">
         <v>223</v>
@@ -11756,7 +11761,7 @@
         <v>279</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J42" s="10" t="s">
         <v>281</v>
@@ -11898,7 +11903,7 @@
         <v>274</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>282</v>
@@ -12036,7 +12041,7 @@
         <v>273</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>283</v>
@@ -12188,7 +12193,7 @@
         <v>276</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>288</v>
@@ -12332,7 +12337,7 @@
         <v>277</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>284</v>
@@ -12456,7 +12461,7 @@
         <v>245</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>330</v>
@@ -12465,10 +12470,10 @@
         <v>550</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J47" s="10" t="s">
         <v>285</v>
@@ -12604,7 +12609,7 @@
         <v>278</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J48" s="10" t="s">
         <v>286</v>
@@ -12760,7 +12765,7 @@
         <v>280</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J49" s="10" t="s">
         <v>287</v>
@@ -12900,13 +12905,13 @@
         <v>399</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>275</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J50" s="10" t="s">
         <v>289</v>
@@ -13035,7 +13040,7 @@
         <v>232</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>266</v>
@@ -13050,7 +13055,7 @@
         <v>272</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J51" s="10" t="s">
         <v>290</v>
@@ -13188,7 +13193,7 @@
         <v>360</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J52" s="10" t="s">
         <v>372</v>
@@ -13908,7 +13913,7 @@
         <v>365</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J57" s="10" t="s">
         <v>377</v>
@@ -14050,7 +14055,7 @@
         <v>366</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J58" s="10" t="s">
         <v>379</v>
@@ -14186,7 +14191,7 @@
         <v>367</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J59" s="10" t="s">
         <v>371</v>
@@ -14466,7 +14471,7 @@
         <v>359</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J61" s="10" t="s">
         <v>380</v>
@@ -14610,7 +14615,7 @@
         <v>409</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J62" s="10" t="s">
         <v>431</v>
@@ -14754,7 +14759,7 @@
         <v>413</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J63" s="10" t="s">
         <v>432</v>
@@ -14896,7 +14901,7 @@
         <v>408</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J64" s="10" t="s">
         <v>436</v>
@@ -15213,19 +15218,19 @@
         <v>229</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>394</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>60</v>
@@ -15364,7 +15369,7 @@
         <v>245</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>392</v>
@@ -15373,10 +15378,10 @@
         <v>417</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J67" s="10" t="s">
         <v>434</v>
@@ -15534,7 +15539,7 @@
         <v>410</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>427</v>
@@ -15674,7 +15679,7 @@
         <v>411</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J69" s="10" t="s">
         <v>428</v>
@@ -15812,7 +15817,7 @@
         <v>412</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J70" s="10" t="s">
         <v>429</v>
@@ -15954,7 +15959,7 @@
         <v>407</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="J71" s="10" t="s">
         <v>430</v>
@@ -16078,7 +16083,7 @@
         <v>454</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J72" s="10" t="s">
         <v>477</v>
@@ -16226,7 +16231,7 @@
         <v>455</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J73" s="10" t="s">
         <v>476</v>
@@ -16380,7 +16385,7 @@
         <v>456</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J74" s="10" t="s">
         <v>474</v>
@@ -16534,7 +16539,7 @@
         <v>457</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J75" s="10" t="s">
         <v>479</v>
@@ -16682,7 +16687,7 @@
         <v>458</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J76" s="10" t="s">
         <v>475</v>
@@ -16832,7 +16837,7 @@
         <v>459</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J77" s="10" t="s">
         <v>473</v>
@@ -16982,7 +16987,7 @@
         <v>460</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J78" s="10" t="s">
         <v>472</v>
@@ -17128,7 +17133,7 @@
         <v>461</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J79" s="10" t="s">
         <v>478</v>
@@ -17406,19 +17411,19 @@
         <v>242</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>471</v>
       </c>
       <c r="G81" s="6" t="s">
+        <v>793</v>
+      </c>
+      <c r="H81" s="6" t="s">
         <v>795</v>
       </c>
-      <c r="H81" s="6" t="s">
-        <v>797</v>
-      </c>
       <c r="I81" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J81" s="10" t="s">
         <v>480</v>
@@ -17592,7 +17597,7 @@
         <v>505</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J82" s="10" t="s">
         <v>512</v>
@@ -17730,19 +17735,19 @@
         <v>240</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>490</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="I83" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J83" s="10" t="s">
         <v>513</v>
@@ -17875,7 +17880,7 @@
         <v>229</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>488</v>
@@ -17890,7 +17895,7 @@
         <v>506</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J84" s="10" t="s">
         <v>514</v>
@@ -18042,7 +18047,7 @@
         <v>507</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J85" s="10" t="s">
         <v>515</v>
@@ -18184,7 +18189,7 @@
         <v>370</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>498</v>
@@ -18193,10 +18198,10 @@
         <v>558</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J86" s="10" t="s">
         <v>516</v>
@@ -18320,19 +18325,19 @@
         <v>245</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>493</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J87" s="10" t="s">
         <v>517</v>
@@ -18453,7 +18458,7 @@
         <v>232</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>482</v>
@@ -18468,7 +18473,7 @@
         <v>508</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J88" s="10" t="s">
         <v>518</v>
@@ -18607,7 +18612,7 @@
         <v>232</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>484</v>
@@ -18622,7 +18627,7 @@
         <v>509</v>
       </c>
       <c r="I89" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J89" s="10" t="s">
         <v>519</v>
@@ -18757,7 +18762,7 @@
         <v>232</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>485</v>
@@ -18772,7 +18777,7 @@
         <v>510</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J90" s="10" t="s">
         <v>520</v>
@@ -18928,7 +18933,7 @@
         <v>511</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J91" s="10" t="s">
         <v>521</v>
@@ -19068,7 +19073,7 @@
         <v>559</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J92" s="10" t="s">
         <v>576</v>
@@ -19214,7 +19219,7 @@
         <v>561</v>
       </c>
       <c r="I93" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J93" s="10" t="s">
         <v>575</v>
@@ -19372,7 +19377,7 @@
         <v>560</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J94" s="10" t="s">
         <v>574</v>
@@ -19524,7 +19529,7 @@
         <v>562</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J95" s="10" t="s">
         <v>567</v>
@@ -19678,7 +19683,7 @@
         <v>563</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J96" s="10" t="s">
         <v>568</v>
@@ -19824,7 +19829,7 @@
         <v>566</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J97" s="10" t="s">
         <v>569</v>
@@ -19968,7 +19973,7 @@
         <v>564</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J98" s="10" t="s">
         <v>583</v>
@@ -20110,7 +20115,7 @@
         <v>565</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J99" s="10" t="s">
         <v>571</v>
@@ -20234,7 +20239,7 @@
         <v>369</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>577</v>
@@ -20243,13 +20248,13 @@
         <v>580</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="K100" s="3">
         <v>4</v>
@@ -20378,19 +20383,19 @@
         <v>369</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>582</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="I101" s="6" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="J101" s="10" t="s">
         <v>573</v>
@@ -20521,25 +20526,25 @@
         <v>232</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E102" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="G102" s="6" t="s">
         <v>616</v>
       </c>
-      <c r="F102" s="6" t="s">
+      <c r="H102" s="6" t="s">
         <v>615</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>618</v>
-      </c>
-      <c r="H102" s="6" t="s">
-        <v>617</v>
       </c>
       <c r="I102" s="6" t="s">
         <v>343</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K102" s="3">
         <v>4</v>
@@ -20662,22 +20667,22 @@
         <v>369</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J103" s="10" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="K103" s="3">
         <v>2</v>
@@ -20804,22 +20809,22 @@
         <v>243</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="K104" s="3">
         <v>4</v>
@@ -20948,22 +20953,22 @@
         <v>243</v>
       </c>
       <c r="E105" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="H105" s="6" t="s">
         <v>620</v>
       </c>
-      <c r="F105" s="6" t="s">
-        <v>606</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>625</v>
-      </c>
-      <c r="H105" s="6" t="s">
-        <v>622</v>
-      </c>
       <c r="I105" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="K105" s="3">
         <v>3</v>
@@ -21094,22 +21099,22 @@
         <v>369</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="I106" s="6" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K106" s="3">
         <v>3</v>
@@ -21230,22 +21235,22 @@
         <v>369</v>
       </c>
       <c r="E107" s="6" t="s">
+        <v>762</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="H107" s="6" t="s">
         <v>764</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>636</v>
-      </c>
-      <c r="G107" s="6" t="s">
-        <v>627</v>
-      </c>
-      <c r="H107" s="6" t="s">
-        <v>766</v>
       </c>
       <c r="I107" s="6" t="s">
         <v>248</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="K107" s="3">
         <v>2</v>
@@ -21368,22 +21373,22 @@
         <v>369</v>
       </c>
       <c r="E108" s="6" t="s">
+        <v>763</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="H108" s="6" t="s">
         <v>765</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>628</v>
-      </c>
-      <c r="H108" s="6" t="s">
-        <v>767</v>
       </c>
       <c r="I108" s="6" t="s">
         <v>335</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="K108" s="3">
         <v>3</v>
@@ -21504,22 +21509,22 @@
         <v>369</v>
       </c>
       <c r="E109" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="H109" s="6" t="s">
         <v>621</v>
-      </c>
-      <c r="F109" s="6" t="s">
-        <v>607</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>629</v>
-      </c>
-      <c r="H109" s="6" t="s">
-        <v>623</v>
       </c>
       <c r="I109" s="6" t="s">
         <v>522</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="K109" s="3">
         <v>2</v>
@@ -21640,22 +21645,22 @@
         <v>369</v>
       </c>
       <c r="E110" s="6" t="s">
+        <v>766</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="G110" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="H110" s="6" t="s">
         <v>768</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>631</v>
-      </c>
-      <c r="H110" s="6" t="s">
-        <v>770</v>
       </c>
       <c r="I110" s="6" t="s">
         <v>261</v>
       </c>
       <c r="J110" s="10" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="K110" s="3">
         <v>3</v>
@@ -21779,25 +21784,25 @@
         <v>229</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E111" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="H111" s="6" t="s">
         <v>611</v>
       </c>
-      <c r="F111" s="6" t="s">
-        <v>635</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>612</v>
-      </c>
-      <c r="H111" s="6" t="s">
-        <v>613</v>
-      </c>
       <c r="I111" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J111" s="10" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="K111" s="3">
         <v>5</v>
@@ -21941,25 +21946,25 @@
         <v>229</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E112" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="H112" s="6" t="s">
         <v>769</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>660</v>
-      </c>
-      <c r="G112" s="6" t="s">
-        <v>677</v>
-      </c>
-      <c r="H112" s="6" t="s">
-        <v>771</v>
       </c>
       <c r="I112" s="6" t="s">
         <v>45</v>
       </c>
       <c r="J112" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K112" s="3">
         <v>3</v>
@@ -22094,22 +22099,22 @@
         <v>242</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I113" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="K113" s="3">
         <v>4</v>
@@ -22253,25 +22258,25 @@
         <v>229</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="I114" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="K114" s="3">
         <v>3</v>
@@ -22403,25 +22408,25 @@
         <v>229</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="H115" s="6" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="I115" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="K115" s="3">
         <v>4</v>
@@ -22551,25 +22556,25 @@
         <v>229</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="I116" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="K116" s="3">
         <v>3</v>
@@ -22710,22 +22715,22 @@
         <v>243</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H117" s="6" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I117" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J117" s="10" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="K117" s="3">
         <v>3</v>
@@ -22858,22 +22863,22 @@
         <v>369</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H118" s="6" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="I118" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="K118" s="3">
         <v>3</v>
@@ -23002,22 +23007,22 @@
         <v>369</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="I119" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J119" s="10" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="K119" s="3">
         <v>3</v>
@@ -23147,25 +23152,25 @@
         <v>232</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I120" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="K120" s="3">
         <v>5</v>
@@ -23298,22 +23303,22 @@
         <v>240</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="I121" s="6" t="s">
         <v>524</v>
       </c>
       <c r="J121" s="10" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="K121" s="3">
         <v>5</v>
@@ -23452,22 +23457,22 @@
         <v>245</v>
       </c>
       <c r="E122" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="F122" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="F122" s="6" t="s">
-        <v>715</v>
-      </c>
       <c r="G122" s="6" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="I122" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="K122" s="3">
         <v>1</v>
@@ -23590,22 +23595,22 @@
         <v>245</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="H123" s="6" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="J123" s="10" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="K123" s="3">
         <v>3</v>
@@ -23732,22 +23737,22 @@
         <v>370</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="H124" s="6" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="I124" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J124" s="10" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="K124" s="3">
         <v>3</v>
@@ -23874,22 +23879,22 @@
         <v>370</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="H125" s="6" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="I125" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="K125" s="3">
         <v>3</v>
@@ -24016,22 +24021,22 @@
         <v>243</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="H126" s="6" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="I126" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J126" s="10" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="K126" s="3">
         <v>4</v>
@@ -24162,22 +24167,22 @@
         <v>369</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="H127" s="6" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="I127" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J127" s="10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="K127" s="3">
         <v>3</v>
@@ -24307,25 +24312,25 @@
         <v>229</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="H128" s="6" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="I128" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J128" s="10" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="K128" s="3">
         <v>4</v>
@@ -24450,22 +24455,22 @@
         <v>244</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H129" s="6" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I129" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J129" s="10" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="K129" s="3">
         <v>3</v>
@@ -24604,22 +24609,22 @@
         <v>246</v>
       </c>
       <c r="E130" s="6" t="s">
+        <v>696</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>697</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="H130" s="6" t="s">
         <v>698</v>
-      </c>
-      <c r="F130" s="6" t="s">
-        <v>699</v>
-      </c>
-      <c r="G130" s="6" t="s">
-        <v>701</v>
-      </c>
-      <c r="H130" s="6" t="s">
-        <v>700</v>
       </c>
       <c r="I130" s="6" t="s">
         <v>487</v>
       </c>
       <c r="J130" s="10" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="K130" s="3">
         <v>3</v>
@@ -24752,22 +24757,22 @@
         <v>424</v>
       </c>
       <c r="E131" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="G131" s="6" t="s">
         <v>723</v>
       </c>
-      <c r="F131" s="6" t="s">
-        <v>697</v>
-      </c>
-      <c r="G131" s="6" t="s">
-        <v>725</v>
-      </c>
       <c r="H131" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="I131" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J131" s="10" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="K131" s="3">
         <v>5</v>
@@ -24894,22 +24899,22 @@
         <v>242</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="H132" s="6" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="I132" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J132" s="10" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="K132" s="3">
         <v>5</v>
@@ -25057,25 +25062,25 @@
         <v>229</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I133" s="6" t="s">
         <v>43</v>
       </c>
       <c r="J133" s="10" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="K133" s="3">
         <v>5</v>
@@ -25218,22 +25223,22 @@
         <v>243</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="H134" s="6" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="I134" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J134" s="10" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="K134" s="3">
         <v>2</v>
@@ -25368,22 +25373,22 @@
         <v>243</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="I135" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J135" s="10" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="K135" s="3">
         <v>3</v>
@@ -25506,22 +25511,22 @@
         <v>370</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F136" s="6" t="s">
+        <v>831</v>
+      </c>
+      <c r="G136" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="G136" s="6" t="s">
-        <v>835</v>
-      </c>
       <c r="H136" s="6" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="I136" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J136" s="10" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="K136" s="3">
         <v>3</v>
@@ -25648,22 +25653,22 @@
         <v>245</v>
       </c>
       <c r="E137" s="6" t="s">
+        <v>849</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="G137" s="6" t="s">
         <v>851</v>
       </c>
-      <c r="F137" s="6" t="s">
-        <v>820</v>
-      </c>
-      <c r="G137" s="6" t="s">
-        <v>853</v>
-      </c>
       <c r="H137" s="6" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="I137" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J137" s="10" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="K137" s="3">
         <v>4</v>
@@ -25796,22 +25801,22 @@
         <v>245</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="I138" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J138" s="10" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="K138" s="3">
         <v>3</v>
@@ -25942,22 +25947,22 @@
         <v>424</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F139" s="6" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G139" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="H139" s="6" t="s">
         <v>809</v>
       </c>
-      <c r="H139" s="6" t="s">
-        <v>811</v>
-      </c>
       <c r="I139" s="6" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="J139" s="10" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="K139" s="3">
         <v>5</v>
@@ -26098,22 +26103,22 @@
         <v>241</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F140" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="H140" s="6" t="s">
         <v>822</v>
-      </c>
-      <c r="G140" s="6" t="s">
-        <v>823</v>
-      </c>
-      <c r="H140" s="6" t="s">
-        <v>824</v>
       </c>
       <c r="I140" s="6" t="s">
         <v>386</v>
       </c>
       <c r="J140" s="10" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="K140" s="3">
         <v>1</v>
@@ -26240,22 +26245,22 @@
         <v>240</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F141" s="6" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="H141" s="6" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I141" s="6" t="s">
         <v>33</v>
       </c>
       <c r="J141" s="10" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="K141" s="3">
         <v>4</v>
@@ -26390,22 +26395,22 @@
         <v>370</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="H142" s="6" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="I142" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J142" s="10" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="K142" s="3">
         <v>1</v>
@@ -26532,22 +26537,22 @@
         <v>369</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="H143" s="6" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="I143" s="6" t="s">
         <v>339</v>
       </c>
       <c r="J143" s="10" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="K143" s="3">
         <v>2</v>
@@ -26666,22 +26671,22 @@
         <v>244</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F144" s="6" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="H144" s="6" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="I144" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J144" s="10" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="K144" s="3">
         <v>3</v>
@@ -26815,19 +26820,19 @@
         <v>159</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G145" s="6" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="H145" s="6" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I145" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J145" s="10" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="K145" s="3">
         <v>3</v>
@@ -26961,19 +26966,19 @@
         <v>133</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="H146" s="6" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="I146" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J146" s="10" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="K146" s="3">
         <v>4</v>
@@ -27094,22 +27099,22 @@
         <v>242</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="H147" s="6" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I147" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J147" s="10" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="K147" s="3">
         <v>4</v>
@@ -27245,25 +27250,25 @@
         <v>232</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="H148" s="6" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="I148" s="6" t="s">
         <v>343</v>
       </c>
       <c r="J148" s="10" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="K148" s="3">
         <v>5</v>
@@ -27388,22 +27393,22 @@
         <v>424</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H149" s="6" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="I149" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J149" s="10" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="K149" s="3">
         <v>5</v>
@@ -27532,22 +27537,22 @@
         <v>240</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="F150" s="6" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G150" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="H150" s="6" t="s">
         <v>861</v>
       </c>
-      <c r="H150" s="6" t="s">
-        <v>863</v>
-      </c>
       <c r="I150" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J150" s="10" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="K150" s="3">
         <v>3</v>
@@ -27688,22 +27693,22 @@
         <v>240</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F151" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="G151" s="6" t="s">
         <v>860</v>
       </c>
-      <c r="G151" s="6" t="s">
+      <c r="H151" s="6" t="s">
         <v>862</v>
       </c>
-      <c r="H151" s="6" t="s">
-        <v>864</v>
-      </c>
       <c r="I151" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J151" s="10" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="K151" s="3">
         <v>5</v>
@@ -27836,22 +27841,22 @@
         <v>369</v>
       </c>
       <c r="E152" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="G152" s="6" t="s">
         <v>924</v>
       </c>
-      <c r="F152" s="6" t="s">
-        <v>937</v>
-      </c>
-      <c r="G152" s="6" t="s">
+      <c r="H152" s="6" t="s">
         <v>926</v>
       </c>
-      <c r="H152" s="6" t="s">
-        <v>928</v>
-      </c>
       <c r="I152" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J152" s="10" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="K152" s="3">
         <v>2</v>
@@ -27970,22 +27975,22 @@
         <v>369</v>
       </c>
       <c r="E153" s="6" t="s">
+        <v>923</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>936</v>
+      </c>
+      <c r="G153" s="6" t="s">
         <v>925</v>
       </c>
-      <c r="F153" s="6" t="s">
-        <v>938</v>
-      </c>
-      <c r="G153" s="6" t="s">
+      <c r="H153" s="6" t="s">
         <v>927</v>
       </c>
-      <c r="H153" s="6" t="s">
-        <v>929</v>
-      </c>
       <c r="I153" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J153" s="10" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="K153" s="3">
         <v>2</v>
@@ -28106,22 +28111,22 @@
         <v>369</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="F154" s="6" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="G154" s="6" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="H154" s="6" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="I154" s="6" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="J154" s="10" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="K154" s="3">
         <v>4</v>
@@ -28242,22 +28247,22 @@
         <v>369</v>
       </c>
       <c r="E155" s="6" t="s">
+        <v>918</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="G155" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="H155" s="6" t="s">
+        <v>929</v>
+      </c>
+      <c r="I155" s="6" t="s">
         <v>920</v>
       </c>
-      <c r="F155" s="6" t="s">
-        <v>940</v>
-      </c>
-      <c r="G155" s="6" t="s">
-        <v>921</v>
-      </c>
-      <c r="H155" s="6" t="s">
-        <v>931</v>
-      </c>
-      <c r="I155" s="6" t="s">
-        <v>922</v>
-      </c>
       <c r="J155" s="10" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="K155" s="3">
         <v>4</v>
@@ -28386,22 +28391,22 @@
         <v>245</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="F156" s="6" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="G156" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="H156" s="6" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="I156" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J156" s="10" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="K156" s="3">
         <v>3</v>
@@ -28542,22 +28547,22 @@
         <v>244</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F157" s="6" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G157" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H157" s="6" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="I157" s="6" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="J157" s="10" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="K157" s="3">
         <v>4</v>
@@ -28696,22 +28701,22 @@
         <v>244</v>
       </c>
       <c r="E158" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="G158" s="6" t="s">
         <v>954</v>
       </c>
-      <c r="F158" s="6" t="s">
+      <c r="H158" s="6" t="s">
         <v>955</v>
       </c>
-      <c r="G158" s="6" t="s">
-        <v>956</v>
-      </c>
-      <c r="H158" s="6" t="s">
-        <v>957</v>
-      </c>
       <c r="I158" s="6" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="J158" s="10" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="K158" s="3">
         <v>4</v>
@@ -28853,25 +28858,25 @@
         <v>232</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F159" s="6" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="G159" s="6" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="H159" s="6" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="I159" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J159" s="10" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="K159" s="3">
         <v>4</v>
@@ -28996,22 +29001,22 @@
         <v>246</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F160" s="6" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="G160" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="H160" s="6" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="I160" s="6" t="s">
         <v>487</v>
       </c>
       <c r="J160" s="10" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="K160" s="3">
         <v>4</v>
@@ -29149,25 +29154,25 @@
         <v>232</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F161" s="6" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G161" s="6" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="H161" s="6" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="I161" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J161" s="10" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="K161" s="3">
         <v>5</v>
@@ -29297,7 +29302,7 @@
       <c r="D162" s="4"/>
       <c r="E162" s="6"/>
       <c r="F162" s="6" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="G162" s="6"/>
       <c r="H162" s="6"/>
@@ -29397,22 +29402,22 @@
         <v>226</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E163" s="6" t="s">
+        <v>948</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="G163" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="H163" s="6" t="s">
         <v>950</v>
       </c>
-      <c r="F163" s="6" t="s">
-        <v>943</v>
-      </c>
-      <c r="G163" s="6" t="s">
+      <c r="I163" s="6" t="s">
         <v>951</v>
-      </c>
-      <c r="H163" s="6" t="s">
-        <v>952</v>
-      </c>
-      <c r="I163" s="6" t="s">
-        <v>953</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="3"/>
@@ -29508,7 +29513,7 @@
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
       <c r="E164" s="6" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
@@ -29608,7 +29613,7 @@
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="6" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
@@ -29708,7 +29713,7 @@
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="6" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
@@ -29808,7 +29813,7 @@
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="6" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
@@ -29908,7 +29913,7 @@
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="6" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
@@ -30008,7 +30013,7 @@
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="6" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
@@ -30298,16 +30303,16 @@
     </row>
     <row r="172" spans="1:55" x14ac:dyDescent="0.15">
       <c r="E172" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="173" spans="1:55" x14ac:dyDescent="0.15">
@@ -30339,7 +30344,7 @@
     </row>
     <row r="179" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E179" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="J179" s="1" t="s">
         <v>187</v>
@@ -30363,7 +30368,7 @@
     </row>
     <row r="182" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E182" s="1" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>190</v>
@@ -30387,7 +30392,7 @@
     </row>
     <row r="185" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E185" s="1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="J185" s="1" t="s">
         <v>193</v>
@@ -30403,7 +30408,7 @@
     </row>
     <row r="187" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E187" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="J187" s="1" t="s">
         <v>195</v>
@@ -30411,7 +30416,7 @@
     </row>
     <row r="188" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E188" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="J188" s="1" t="s">
         <v>196</v>
@@ -30435,7 +30440,7 @@
     </row>
     <row r="191" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E191" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="J191" s="1" t="s">
         <v>199</v>
@@ -30499,7 +30504,7 @@
     </row>
     <row r="199" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E199" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="J199" s="1" t="s">
         <v>207</v>
@@ -30515,7 +30520,7 @@
     </row>
     <row r="201" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E201" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="J201" s="1" t="s">
         <v>209</v>
@@ -30547,7 +30552,7 @@
     </row>
     <row r="205" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E205" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="J205" s="1" t="s">
         <v>213</v>
@@ -30619,7 +30624,7 @@
     </row>
     <row r="214" spans="5:10" x14ac:dyDescent="0.15">
       <c r="E214" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="J214" s="1" t="s">
         <v>222</v>

</xml_diff>